<commit_message>
Update RVs with RuleSets
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cv-gender.xlsx
+++ b/output/StructureDefinition-cv-gender.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$99</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3387" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3849" uniqueCount="582">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-28T16:37:13+02:00</t>
+    <t>2023-03-28T22:15:03+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Das Geschlecht einer Person.</t>
+    <t>Dieses abstrakte Profil beschreibt die 'Geschlechtskategorie, als Merkmal von Personen'.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -632,7 +632,7 @@
     <t>Observation.category</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
   <si>
     <t xml:space="preserve">CodeableConcept
@@ -676,13 +676,13 @@
     <t>FiveWs.class</t>
   </si>
   <si>
-    <t>Observation.category:Gender</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Observation.category:Gender.id</t>
+    <t>Observation.category:Gender_UMLS</t>
+  </si>
+  <si>
+    <t>Gender_UMLS</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_UMLS.id</t>
   </si>
   <si>
     <t>Observation.category.id</t>
@@ -701,7 +701,7 @@
     <t>Element.id</t>
   </si>
   <si>
-    <t>Observation.category:Gender.extension</t>
+    <t>Observation.category:Gender_UMLS.extension</t>
   </si>
   <si>
     <t>Observation.category.extension</t>
@@ -713,7 +713,7 @@
     <t>Element.extension</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding</t>
+    <t>Observation.category:Gender_UMLS.coding</t>
   </si>
   <si>
     <t>Observation.category.coding</t>
@@ -744,19 +744,19 @@
     <t>union(., ./translation)</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.id</t>
+    <t>Observation.category:Gender_UMLS.coding.id</t>
   </si>
   <si>
     <t>Observation.category.coding.id</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.extension</t>
+    <t>Observation.category:Gender_UMLS.coding.extension</t>
   </si>
   <si>
     <t>Observation.category.coding.extension</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.system</t>
+    <t>Observation.category:Gender_UMLS.coding.system</t>
   </si>
   <si>
     <t>Observation.category.coding.system</t>
@@ -774,7 +774,7 @@
     <t>Need to be unambiguous about the source of the definition of the symbol.</t>
   </si>
   <si>
-    <t>http://snomed.info/sct</t>
+    <t>http://terminology.hl7.org/CodeSystem/umls</t>
   </si>
   <si>
     <t>Coding.system</t>
@@ -786,7 +786,7 @@
     <t>./codeSystem</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.version</t>
+    <t>Observation.category:Gender_UMLS.coding.version</t>
   </si>
   <si>
     <t>Observation.category.coding.version</t>
@@ -810,7 +810,7 @@
     <t>./codeSystemVersion</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.code</t>
+    <t>Observation.category:Gender_UMLS.coding.code</t>
   </si>
   <si>
     <t>Observation.category.coding.code</t>
@@ -828,7 +828,7 @@
     <t>Need to refer to a particular code in the system.</t>
   </si>
   <si>
-    <t>263495000</t>
+    <t>C0079399</t>
   </si>
   <si>
     <t>Coding.code</t>
@@ -840,7 +840,7 @@
     <t>./code</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.display</t>
+    <t>Observation.category:Gender_UMLS.coding.display</t>
   </si>
   <si>
     <t>Observation.category.coding.display</t>
@@ -864,7 +864,7 @@
     <t>CV.displayName</t>
   </si>
   <si>
-    <t>Observation.category:Gender.coding.userSelected</t>
+    <t>Observation.category:Gender_UMLS.coding.userSelected</t>
   </si>
   <si>
     <t>Observation.category.coding.userSelected</t>
@@ -895,7 +895,7 @@
     <t>CD.codingRationale</t>
   </si>
   <si>
-    <t>Observation.category:Gender.text</t>
+    <t>Observation.category:Gender_UMLS.text</t>
   </si>
   <si>
     <t>Observation.category.text</t>
@@ -922,6 +922,51 @@
     <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
+    <t>Observation.category:Gender_SNOMED</t>
+  </si>
+  <si>
+    <t>Gender_SNOMED</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.id</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.extension</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.id</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.extension</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.system</t>
+  </si>
+  <si>
+    <t>http://snomed.info/sct</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.version</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.code</t>
+  </si>
+  <si>
+    <t>263495000</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.display</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.coding.userSelected</t>
+  </si>
+  <si>
+    <t>Observation.category:Gender_SNOMED.text</t>
+  </si>
+  <si>
     <t>Observation.category:Persons</t>
   </si>
   <si>
@@ -986,9 +1031,6 @@
   </si>
   <si>
     <t>Observation.category:NominalScale.coding.system</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/CodeSystem/umls</t>
   </si>
   <si>
     <t>Observation.category:NominalScale.coding.version</t>
@@ -2104,7 +2146,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP87"/>
+  <dimension ref="A1:AP99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2113,9 +2155,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="51.6015625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="55.3984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="43.60546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.1875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="16.984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -6191,7 +6233,7 @@
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" t="s" s="2">
-        <v>243</v>
+        <v>300</v>
       </c>
       <c r="S34" t="s" s="2">
         <v>82</v>
@@ -6268,7 +6310,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B35" t="s" s="2">
         <v>248</v>
@@ -6388,7 +6430,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B36" t="s" s="2">
         <v>256</v>
@@ -6433,7 +6475,7 @@
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="S36" t="s" s="2">
         <v>82</v>
@@ -6510,7 +6552,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B37" t="s" s="2">
         <v>266</v>
@@ -6632,7 +6674,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B38" t="s" s="2">
         <v>274</v>
@@ -6754,7 +6796,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B39" t="s" s="2">
         <v>284</v>
@@ -6876,13 +6918,13 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B40" t="s" s="2">
         <v>196</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D40" t="s" s="2">
         <v>82</v>
@@ -7000,7 +7042,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B41" t="s" s="2">
         <v>214</v>
@@ -7118,7 +7160,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B42" t="s" s="2">
         <v>220</v>
@@ -7238,7 +7280,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B43" t="s" s="2">
         <v>224</v>
@@ -7360,7 +7402,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B44" t="s" s="2">
         <v>234</v>
@@ -7478,7 +7520,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B45" t="s" s="2">
         <v>236</v>
@@ -7598,7 +7640,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B46" t="s" s="2">
         <v>238</v>
@@ -7643,7 +7685,7 @@
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" t="s" s="2">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="S46" t="s" s="2">
         <v>82</v>
@@ -8331,11 +8373,13 @@
         <v>321</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>196</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>322</v>
+      </c>
       <c r="D52" t="s" s="2">
-        <v>322</v>
+        <v>82</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
@@ -8345,28 +8389,28 @@
         <v>92</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I52" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K52" t="s" s="2">
         <v>198</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>323</v>
+        <v>199</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>324</v>
+        <v>200</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>325</v>
+        <v>201</v>
       </c>
       <c r="O52" t="s" s="2">
-        <v>326</v>
+        <v>202</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>82</v>
@@ -8391,13 +8435,13 @@
         <v>82</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>327</v>
+        <v>119</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>328</v>
+        <v>203</v>
       </c>
       <c r="Z52" t="s" s="2">
-        <v>329</v>
+        <v>204</v>
       </c>
       <c r="AA52" t="s" s="2">
         <v>82</v>
@@ -8415,13 +8459,13 @@
         <v>82</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>321</v>
+        <v>196</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>104</v>
@@ -8430,30 +8474,30 @@
         <v>105</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>330</v>
+        <v>82</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>331</v>
+        <v>82</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>332</v>
+        <v>208</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>333</v>
+        <v>209</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>334</v>
+        <v>210</v>
       </c>
       <c r="AP52" t="s" s="2">
-        <v>335</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>336</v>
+        <v>214</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8473,23 +8517,19 @@
         <v>82</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>337</v>
+        <v>215</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>338</v>
+        <v>216</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="O53" t="s" s="2">
-        <v>341</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
         <v>82</v>
       </c>
@@ -8537,7 +8577,7 @@
         <v>82</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>336</v>
+        <v>218</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>80</v>
@@ -8546,25 +8586,25 @@
         <v>92</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>342</v>
+        <v>82</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>343</v>
+        <v>82</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>344</v>
+        <v>113</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>345</v>
+        <v>82</v>
       </c>
       <c r="AP53" t="s" s="2">
         <v>82</v>
@@ -8572,14 +8612,14 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>346</v>
+        <v>220</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -8595,19 +8635,19 @@
         <v>82</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>347</v>
+        <v>140</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>348</v>
+        <v>141</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>349</v>
+        <v>221</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>350</v>
+        <v>143</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8645,19 +8685,19 @@
         <v>82</v>
       </c>
       <c r="AB54" t="s" s="2">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AC54" t="s" s="2">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD54" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>346</v>
+        <v>222</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>80</v>
@@ -8669,7 +8709,7 @@
         <v>104</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>82</v>
@@ -8678,13 +8718,13 @@
         <v>82</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>332</v>
+        <v>82</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>351</v>
+        <v>106</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>345</v>
+        <v>82</v>
       </c>
       <c r="AP54" t="s" s="2">
         <v>82</v>
@@ -8692,21 +8732,21 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>352</v>
+        <v>224</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>353</v>
+        <v>82</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>82</v>
@@ -8718,19 +8758,19 @@
         <v>93</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>354</v>
+        <v>225</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>355</v>
+        <v>226</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>356</v>
+        <v>227</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>357</v>
+        <v>228</v>
       </c>
       <c r="O55" t="s" s="2">
-        <v>358</v>
+        <v>229</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>82</v>
@@ -8779,34 +8819,34 @@
         <v>82</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>352</v>
+        <v>230</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>359</v>
+        <v>82</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>360</v>
+        <v>231</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>361</v>
+        <v>232</v>
       </c>
       <c r="AO55" t="s" s="2">
-        <v>362</v>
+        <v>82</v>
       </c>
       <c r="AP55" t="s" s="2">
         <v>82</v>
@@ -8814,14 +8854,14 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>363</v>
+        <v>326</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>363</v>
+        <v>234</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>364</v>
+        <v>82</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8837,23 +8877,19 @@
         <v>82</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>365</v>
+        <v>215</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>366</v>
+        <v>216</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="O56" t="s" s="2">
-        <v>369</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
         <v>82</v>
       </c>
@@ -8901,7 +8937,7 @@
         <v>82</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>363</v>
+        <v>218</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>80</v>
@@ -8910,25 +8946,25 @@
         <v>92</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>370</v>
+        <v>82</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>371</v>
+        <v>82</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>372</v>
+        <v>113</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>373</v>
+        <v>82</v>
       </c>
       <c r="AP56" t="s" s="2">
         <v>82</v>
@@ -8936,21 +8972,21 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>374</v>
+        <v>327</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>374</v>
+        <v>236</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>82</v>
@@ -8959,19 +8995,19 @@
         <v>82</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>375</v>
+        <v>140</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>376</v>
+        <v>141</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>377</v>
+        <v>221</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>378</v>
+        <v>143</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -9009,31 +9045,31 @@
         <v>82</v>
       </c>
       <c r="AB57" t="s" s="2">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AC57" t="s" s="2">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD57" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>374</v>
+        <v>222</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>82</v>
@@ -9042,13 +9078,13 @@
         <v>82</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>379</v>
+        <v>82</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>380</v>
+        <v>106</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>381</v>
+        <v>82</v>
       </c>
       <c r="AP57" t="s" s="2">
         <v>82</v>
@@ -9056,10 +9092,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>382</v>
+        <v>328</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>382</v>
+        <v>238</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -9067,10 +9103,10 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>82</v>
@@ -9082,26 +9118,26 @@
         <v>93</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>383</v>
+        <v>108</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>384</v>
+        <v>239</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>385</v>
+        <v>240</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>168</v>
+        <v>241</v>
       </c>
       <c r="O58" t="s" s="2">
-        <v>386</v>
+        <v>242</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" t="s" s="2">
-        <v>82</v>
+        <v>243</v>
       </c>
       <c r="S58" t="s" s="2">
         <v>82</v>
@@ -9143,34 +9179,34 @@
         <v>82</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>382</v>
+        <v>244</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>387</v>
+        <v>82</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>388</v>
+        <v>245</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>389</v>
+        <v>246</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>390</v>
+        <v>82</v>
       </c>
       <c r="AP58" t="s" s="2">
         <v>82</v>
@@ -9178,10 +9214,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>391</v>
+        <v>329</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>391</v>
+        <v>248</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9204,20 +9240,18 @@
         <v>93</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>392</v>
+        <v>215</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>393</v>
+        <v>249</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>394</v>
+        <v>250</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="O59" t="s" s="2">
-        <v>396</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>82</v>
       </c>
@@ -9265,7 +9299,7 @@
         <v>82</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>391</v>
+        <v>252</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>80</v>
@@ -9274,7 +9308,7 @@
         <v>92</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>397</v>
+        <v>104</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>105</v>
@@ -9283,27 +9317,27 @@
         <v>82</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>398</v>
+        <v>82</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>399</v>
+        <v>253</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>400</v>
+        <v>254</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP59" t="s" s="2">
-        <v>401</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>402</v>
+        <v>330</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>402</v>
+        <v>256</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9311,7 +9345,7 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>92</v>
@@ -9323,29 +9357,29 @@
         <v>82</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>198</v>
+        <v>115</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>403</v>
+        <v>257</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>404</v>
+        <v>258</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>405</v>
+        <v>259</v>
       </c>
       <c r="O60" t="s" s="2">
-        <v>406</v>
+        <v>260</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" t="s" s="2">
-        <v>82</v>
+        <v>331</v>
       </c>
       <c r="S60" t="s" s="2">
         <v>82</v>
@@ -9363,13 +9397,13 @@
         <v>82</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>407</v>
+        <v>82</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>408</v>
+        <v>82</v>
       </c>
       <c r="Z60" t="s" s="2">
-        <v>409</v>
+        <v>82</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>82</v>
@@ -9387,7 +9421,7 @@
         <v>82</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>402</v>
+        <v>262</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>80</v>
@@ -9396,7 +9430,7 @@
         <v>92</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>410</v>
+        <v>104</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>105</v>
@@ -9408,10 +9442,10 @@
         <v>82</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>106</v>
+        <v>263</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>411</v>
+        <v>264</v>
       </c>
       <c r="AO60" t="s" s="2">
         <v>82</v>
@@ -9422,21 +9456,21 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>412</v>
+        <v>332</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>412</v>
+        <v>266</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>413</v>
+        <v>82</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>82</v>
@@ -9445,22 +9479,22 @@
         <v>82</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>414</v>
+        <v>267</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>415</v>
+        <v>268</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>416</v>
+        <v>259</v>
       </c>
       <c r="O61" t="s" s="2">
-        <v>417</v>
+        <v>269</v>
       </c>
       <c r="P61" t="s" s="2">
         <v>82</v>
@@ -9485,13 +9519,13 @@
         <v>82</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>407</v>
+        <v>82</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>418</v>
+        <v>82</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>419</v>
+        <v>82</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>82</v>
@@ -9509,13 +9543,13 @@
         <v>82</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>412</v>
+        <v>270</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>104</v>
@@ -9527,27 +9561,27 @@
         <v>82</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>420</v>
+        <v>82</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>421</v>
+        <v>271</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>422</v>
+        <v>272</v>
       </c>
       <c r="AO61" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP61" t="s" s="2">
-        <v>423</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>424</v>
+        <v>333</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>424</v>
+        <v>274</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9558,7 +9592,7 @@
         <v>80</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>82</v>
@@ -9567,22 +9601,22 @@
         <v>82</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>425</v>
+        <v>275</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>426</v>
+        <v>276</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>427</v>
+        <v>277</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>428</v>
+        <v>278</v>
       </c>
       <c r="O62" t="s" s="2">
-        <v>429</v>
+        <v>279</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>82</v>
@@ -9631,13 +9665,13 @@
         <v>82</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>424</v>
+        <v>280</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>104</v>
@@ -9652,10 +9686,10 @@
         <v>82</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>430</v>
+        <v>281</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>431</v>
+        <v>282</v>
       </c>
       <c r="AO62" t="s" s="2">
         <v>82</v>
@@ -9666,10 +9700,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>432</v>
+        <v>334</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>432</v>
+        <v>284</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9689,21 +9723,23 @@
         <v>82</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>433</v>
+        <v>285</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>434</v>
+        <v>286</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>435</v>
-      </c>
-      <c r="O63" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="O63" t="s" s="2">
+        <v>288</v>
+      </c>
       <c r="P63" t="s" s="2">
         <v>82</v>
       </c>
@@ -9727,13 +9763,13 @@
         <v>82</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>327</v>
+        <v>82</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>436</v>
+        <v>82</v>
       </c>
       <c r="Z63" t="s" s="2">
-        <v>437</v>
+        <v>82</v>
       </c>
       <c r="AA63" t="s" s="2">
         <v>82</v>
@@ -9751,7 +9787,7 @@
         <v>82</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>432</v>
+        <v>289</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>80</v>
@@ -9769,35 +9805,35 @@
         <v>82</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>438</v>
+        <v>82</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>439</v>
+        <v>290</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>440</v>
+        <v>291</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP63" t="s" s="2">
-        <v>441</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>442</v>
+        <v>335</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>442</v>
+        <v>335</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>82</v>
+        <v>336</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>92</v>
@@ -9809,22 +9845,22 @@
         <v>82</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K64" t="s" s="2">
         <v>198</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>443</v>
+        <v>337</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>444</v>
+        <v>338</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>445</v>
+        <v>339</v>
       </c>
       <c r="O64" t="s" s="2">
-        <v>446</v>
+        <v>340</v>
       </c>
       <c r="P64" t="s" s="2">
         <v>82</v>
@@ -9849,13 +9885,13 @@
         <v>82</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>447</v>
+        <v>342</v>
       </c>
       <c r="Z64" t="s" s="2">
-        <v>448</v>
+        <v>343</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>82</v>
@@ -9873,10 +9909,10 @@
         <v>82</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>442</v>
+        <v>335</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>92</v>
@@ -9888,30 +9924,30 @@
         <v>105</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>82</v>
+        <v>344</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>82</v>
+        <v>345</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>449</v>
+        <v>346</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>450</v>
+        <v>347</v>
       </c>
       <c r="AO64" t="s" s="2">
-        <v>82</v>
+        <v>348</v>
       </c>
       <c r="AP64" t="s" s="2">
-        <v>82</v>
+        <v>349</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>451</v>
+        <v>350</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>451</v>
+        <v>350</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9931,21 +9967,23 @@
         <v>82</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>452</v>
+        <v>351</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>453</v>
+        <v>352</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>454</v>
+        <v>353</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="O65" s="2"/>
+        <v>354</v>
+      </c>
+      <c r="O65" t="s" s="2">
+        <v>355</v>
+      </c>
       <c r="P65" t="s" s="2">
         <v>82</v>
       </c>
@@ -9993,7 +10031,7 @@
         <v>82</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>451</v>
+        <v>350</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>80</v>
@@ -10008,30 +10046,30 @@
         <v>170</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>82</v>
+        <v>356</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>456</v>
+        <v>82</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>457</v>
+        <v>357</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>458</v>
+        <v>358</v>
       </c>
       <c r="AO65" t="s" s="2">
-        <v>82</v>
+        <v>359</v>
       </c>
       <c r="AP65" t="s" s="2">
-        <v>459</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>460</v>
+        <v>360</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>460</v>
+        <v>360</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -10042,7 +10080,7 @@
         <v>80</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H66" t="s" s="2">
         <v>82</v>
@@ -10051,19 +10089,19 @@
         <v>82</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>461</v>
+        <v>361</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>462</v>
+        <v>362</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>463</v>
+        <v>363</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>464</v>
+        <v>364</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -10113,13 +10151,13 @@
         <v>82</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>460</v>
+        <v>360</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>104</v>
@@ -10131,38 +10169,38 @@
         <v>82</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>465</v>
+        <v>82</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>466</v>
+        <v>346</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>467</v>
+        <v>365</v>
       </c>
       <c r="AO66" t="s" s="2">
-        <v>82</v>
+        <v>359</v>
       </c>
       <c r="AP66" t="s" s="2">
-        <v>468</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>469</v>
+        <v>366</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>469</v>
+        <v>366</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
-        <v>82</v>
+        <v>367</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>82</v>
@@ -10171,22 +10209,22 @@
         <v>82</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>470</v>
+        <v>368</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>471</v>
+        <v>369</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>472</v>
+        <v>370</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>473</v>
+        <v>371</v>
       </c>
       <c r="O67" t="s" s="2">
-        <v>474</v>
+        <v>372</v>
       </c>
       <c r="P67" t="s" s="2">
         <v>82</v>
@@ -10235,34 +10273,34 @@
         <v>82</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>469</v>
+        <v>366</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH67" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI67" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>475</v>
+        <v>170</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>82</v>
+        <v>373</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>476</v>
+        <v>374</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>477</v>
+        <v>375</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>82</v>
+        <v>376</v>
       </c>
       <c r="AP67" t="s" s="2">
         <v>82</v>
@@ -10270,14 +10308,14 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>478</v>
+        <v>377</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>478</v>
+        <v>377</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
-        <v>82</v>
+        <v>378</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" t="s" s="2">
@@ -10293,19 +10331,23 @@
         <v>82</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>215</v>
+        <v>379</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>216</v>
+        <v>380</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
+        <v>381</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="O68" t="s" s="2">
+        <v>383</v>
+      </c>
       <c r="P68" t="s" s="2">
         <v>82</v>
       </c>
@@ -10353,7 +10395,7 @@
         <v>82</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>218</v>
+        <v>377</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>80</v>
@@ -10362,25 +10404,25 @@
         <v>92</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>82</v>
+        <v>384</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>82</v>
+        <v>385</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>113</v>
+        <v>386</v>
       </c>
       <c r="AO68" t="s" s="2">
-        <v>82</v>
+        <v>387</v>
       </c>
       <c r="AP68" t="s" s="2">
         <v>82</v>
@@ -10388,21 +10430,21 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>479</v>
+        <v>388</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>479</v>
+        <v>388</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G69" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H69" t="s" s="2">
         <v>82</v>
@@ -10411,19 +10453,19 @@
         <v>82</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>140</v>
+        <v>389</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>141</v>
+        <v>390</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>221</v>
+        <v>391</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>143</v>
+        <v>392</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -10461,31 +10503,31 @@
         <v>82</v>
       </c>
       <c r="AB69" t="s" s="2">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="AC69" t="s" s="2">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="AD69" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>222</v>
+        <v>388</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>82</v>
@@ -10494,13 +10536,13 @@
         <v>82</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>82</v>
+        <v>393</v>
       </c>
       <c r="AN69" t="s" s="2">
-        <v>106</v>
+        <v>394</v>
       </c>
       <c r="AO69" t="s" s="2">
-        <v>82</v>
+        <v>395</v>
       </c>
       <c r="AP69" t="s" s="2">
         <v>82</v>
@@ -10508,14 +10550,14 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>480</v>
+        <v>396</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>480</v>
+        <v>396</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
-        <v>481</v>
+        <v>82</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" t="s" s="2">
@@ -10528,25 +10570,25 @@
         <v>82</v>
       </c>
       <c r="I70" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J70" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>140</v>
+        <v>397</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>482</v>
+        <v>398</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>483</v>
+        <v>399</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="O70" t="s" s="2">
-        <v>152</v>
+        <v>400</v>
       </c>
       <c r="P70" t="s" s="2">
         <v>82</v>
@@ -10595,7 +10637,7 @@
         <v>82</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>484</v>
+        <v>396</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>80</v>
@@ -10607,22 +10649,22 @@
         <v>104</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>82</v>
+        <v>401</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>82</v>
+        <v>402</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>106</v>
+        <v>403</v>
       </c>
       <c r="AO70" t="s" s="2">
-        <v>82</v>
+        <v>404</v>
       </c>
       <c r="AP70" t="s" s="2">
         <v>82</v>
@@ -10630,10 +10672,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>485</v>
+        <v>405</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>485</v>
+        <v>405</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10653,21 +10695,23 @@
         <v>82</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>486</v>
+        <v>406</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>487</v>
+        <v>407</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>488</v>
+        <v>408</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="O71" s="2"/>
+        <v>409</v>
+      </c>
+      <c r="O71" t="s" s="2">
+        <v>410</v>
+      </c>
       <c r="P71" t="s" s="2">
         <v>82</v>
       </c>
@@ -10715,7 +10759,7 @@
         <v>82</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>485</v>
+        <v>405</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>80</v>
@@ -10724,36 +10768,36 @@
         <v>92</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>490</v>
+        <v>411</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>491</v>
+        <v>105</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>82</v>
+        <v>412</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>492</v>
+        <v>413</v>
       </c>
       <c r="AN71" t="s" s="2">
-        <v>493</v>
+        <v>414</v>
       </c>
       <c r="AO71" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP71" t="s" s="2">
-        <v>82</v>
+        <v>415</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>494</v>
+        <v>416</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>494</v>
+        <v>416</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10776,18 +10820,20 @@
         <v>82</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>486</v>
+        <v>198</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>495</v>
+        <v>417</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>496</v>
+        <v>418</v>
       </c>
       <c r="N72" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="O72" s="2"/>
+        <v>419</v>
+      </c>
+      <c r="O72" t="s" s="2">
+        <v>420</v>
+      </c>
       <c r="P72" t="s" s="2">
         <v>82</v>
       </c>
@@ -10811,13 +10857,13 @@
         <v>82</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>82</v>
+        <v>421</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>82</v>
+        <v>422</v>
       </c>
       <c r="Z72" t="s" s="2">
-        <v>82</v>
+        <v>423</v>
       </c>
       <c r="AA72" t="s" s="2">
         <v>82</v>
@@ -10835,7 +10881,7 @@
         <v>82</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>494</v>
+        <v>416</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>80</v>
@@ -10844,10 +10890,10 @@
         <v>92</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>490</v>
+        <v>424</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>491</v>
+        <v>105</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>82</v>
@@ -10856,10 +10902,10 @@
         <v>82</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>492</v>
+        <v>106</v>
       </c>
       <c r="AN72" t="s" s="2">
-        <v>497</v>
+        <v>425</v>
       </c>
       <c r="AO72" t="s" s="2">
         <v>82</v>
@@ -10870,21 +10916,21 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>498</v>
+        <v>426</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>498</v>
+        <v>426</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
-        <v>82</v>
+        <v>427</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H73" t="s" s="2">
         <v>82</v>
@@ -10899,16 +10945,16 @@
         <v>198</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>499</v>
+        <v>428</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>500</v>
+        <v>429</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>501</v>
+        <v>430</v>
       </c>
       <c r="O73" t="s" s="2">
-        <v>502</v>
+        <v>431</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>82</v>
@@ -10933,13 +10979,13 @@
         <v>82</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>119</v>
+        <v>421</v>
       </c>
       <c r="Y73" t="s" s="2">
-        <v>503</v>
+        <v>432</v>
       </c>
       <c r="Z73" t="s" s="2">
-        <v>504</v>
+        <v>433</v>
       </c>
       <c r="AA73" t="s" s="2">
         <v>82</v>
@@ -10957,13 +11003,13 @@
         <v>82</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>498</v>
+        <v>426</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH73" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI73" t="s" s="2">
         <v>104</v>
@@ -10975,27 +11021,27 @@
         <v>82</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>505</v>
+        <v>434</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>506</v>
+        <v>435</v>
       </c>
       <c r="AN73" t="s" s="2">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="AO73" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP73" t="s" s="2">
-        <v>82</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>507</v>
+        <v>438</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>507</v>
+        <v>438</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -11018,19 +11064,19 @@
         <v>82</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>198</v>
+        <v>439</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>508</v>
+        <v>440</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>509</v>
+        <v>441</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>510</v>
+        <v>442</v>
       </c>
       <c r="O74" t="s" s="2">
-        <v>511</v>
+        <v>443</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>82</v>
@@ -11055,13 +11101,13 @@
         <v>82</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>327</v>
+        <v>82</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>512</v>
+        <v>82</v>
       </c>
       <c r="Z74" t="s" s="2">
-        <v>513</v>
+        <v>82</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>82</v>
@@ -11079,7 +11125,7 @@
         <v>82</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>507</v>
+        <v>438</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>80</v>
@@ -11097,13 +11143,13 @@
         <v>82</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>505</v>
+        <v>82</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>506</v>
+        <v>444</v>
       </c>
       <c r="AN74" t="s" s="2">
-        <v>422</v>
+        <v>445</v>
       </c>
       <c r="AO74" t="s" s="2">
         <v>82</v>
@@ -11114,10 +11160,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>514</v>
+        <v>446</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>514</v>
+        <v>446</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11140,20 +11186,18 @@
         <v>82</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>515</v>
+        <v>198</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>516</v>
+        <v>447</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>517</v>
+        <v>448</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>518</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>519</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
         <v>82</v>
       </c>
@@ -11177,13 +11221,13 @@
         <v>82</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>82</v>
+        <v>341</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>82</v>
+        <v>450</v>
       </c>
       <c r="Z75" t="s" s="2">
-        <v>82</v>
+        <v>451</v>
       </c>
       <c r="AA75" t="s" s="2">
         <v>82</v>
@@ -11201,7 +11245,7 @@
         <v>82</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>514</v>
+        <v>446</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>80</v>
@@ -11213,33 +11257,33 @@
         <v>104</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>520</v>
+        <v>105</v>
       </c>
       <c r="AK75" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>82</v>
+        <v>452</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>521</v>
+        <v>453</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>522</v>
+        <v>454</v>
       </c>
       <c r="AO75" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP75" t="s" s="2">
-        <v>82</v>
+        <v>455</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>523</v>
+        <v>456</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>523</v>
+        <v>456</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -11262,18 +11306,20 @@
         <v>82</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>524</v>
+        <v>457</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>525</v>
+        <v>458</v>
       </c>
       <c r="N76" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="O76" s="2"/>
+        <v>459</v>
+      </c>
+      <c r="O76" t="s" s="2">
+        <v>460</v>
+      </c>
       <c r="P76" t="s" s="2">
         <v>82</v>
       </c>
@@ -11297,13 +11343,13 @@
         <v>82</v>
       </c>
       <c r="X76" t="s" s="2">
-        <v>82</v>
+        <v>341</v>
       </c>
       <c r="Y76" t="s" s="2">
-        <v>82</v>
+        <v>461</v>
       </c>
       <c r="Z76" t="s" s="2">
-        <v>82</v>
+        <v>462</v>
       </c>
       <c r="AA76" t="s" s="2">
         <v>82</v>
@@ -11321,7 +11367,7 @@
         <v>82</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>523</v>
+        <v>456</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>80</v>
@@ -11342,10 +11388,10 @@
         <v>82</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>492</v>
+        <v>463</v>
       </c>
       <c r="AN76" t="s" s="2">
-        <v>526</v>
+        <v>464</v>
       </c>
       <c r="AO76" t="s" s="2">
         <v>82</v>
@@ -11356,10 +11402,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>527</v>
+        <v>465</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>527</v>
+        <v>465</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11370,7 +11416,7 @@
         <v>80</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>82</v>
@@ -11379,19 +11425,19 @@
         <v>82</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>528</v>
+        <v>466</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>529</v>
+        <v>467</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>530</v>
+        <v>468</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>531</v>
+        <v>469</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
@@ -11441,13 +11487,13 @@
         <v>82</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>527</v>
+        <v>465</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>104</v>
@@ -11459,27 +11505,27 @@
         <v>82</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>82</v>
+        <v>470</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>532</v>
+        <v>471</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>533</v>
+        <v>472</v>
       </c>
       <c r="AO77" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP77" t="s" s="2">
-        <v>82</v>
+        <v>473</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>534</v>
+        <v>474</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>534</v>
+        <v>474</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11490,7 +11536,7 @@
         <v>80</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>82</v>
@@ -11499,19 +11545,19 @@
         <v>82</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>535</v>
+        <v>475</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>536</v>
+        <v>476</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>537</v>
+        <v>477</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>538</v>
+        <v>478</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
@@ -11561,13 +11607,13 @@
         <v>82</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>534</v>
+        <v>474</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI78" t="s" s="2">
         <v>104</v>
@@ -11579,27 +11625,27 @@
         <v>82</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>82</v>
+        <v>479</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>532</v>
+        <v>480</v>
       </c>
       <c r="AN78" t="s" s="2">
-        <v>539</v>
+        <v>481</v>
       </c>
       <c r="AO78" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP78" t="s" s="2">
-        <v>82</v>
+        <v>482</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>540</v>
+        <v>483</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>540</v>
+        <v>483</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11619,22 +11665,22 @@
         <v>82</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>541</v>
+        <v>485</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>542</v>
+        <v>486</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>543</v>
+        <v>487</v>
       </c>
       <c r="O79" t="s" s="2">
-        <v>544</v>
+        <v>488</v>
       </c>
       <c r="P79" t="s" s="2">
         <v>82</v>
@@ -11683,7 +11729,7 @@
         <v>82</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>540</v>
+        <v>483</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>80</v>
@@ -11695,7 +11741,7 @@
         <v>104</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>82</v>
+        <v>489</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>82</v>
@@ -11704,10 +11750,10 @@
         <v>82</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>545</v>
+        <v>490</v>
       </c>
       <c r="AN79" t="s" s="2">
-        <v>546</v>
+        <v>491</v>
       </c>
       <c r="AO79" t="s" s="2">
         <v>82</v>
@@ -11718,10 +11764,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>547</v>
+        <v>492</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>547</v>
+        <v>492</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11836,10 +11882,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>548</v>
+        <v>493</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>548</v>
+        <v>493</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11956,14 +12002,14 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>549</v>
+        <v>494</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>549</v>
+        <v>494</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" t="s" s="2">
@@ -11985,10 +12031,10 @@
         <v>140</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="N82" t="s" s="2">
         <v>143</v>
@@ -12043,7 +12089,7 @@
         <v>82</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>80</v>
@@ -12078,10 +12124,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>550</v>
+        <v>499</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>550</v>
+        <v>499</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -12089,7 +12135,7 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>92</v>
@@ -12101,23 +12147,21 @@
         <v>82</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>198</v>
+        <v>500</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>551</v>
+        <v>501</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>552</v>
+        <v>502</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>553</v>
-      </c>
-      <c r="O83" t="s" s="2">
-        <v>326</v>
-      </c>
+        <v>503</v>
+      </c>
+      <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
         <v>82</v>
       </c>
@@ -12141,13 +12185,13 @@
         <v>82</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>327</v>
+        <v>82</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>328</v>
+        <v>82</v>
       </c>
       <c r="Z83" t="s" s="2">
-        <v>329</v>
+        <v>82</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>82</v>
@@ -12165,34 +12209,34 @@
         <v>82</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>550</v>
+        <v>499</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>92</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>104</v>
+        <v>504</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>105</v>
+        <v>505</v>
       </c>
       <c r="AK83" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>554</v>
+        <v>82</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>332</v>
+        <v>506</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>333</v>
+        <v>507</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>334</v>
+        <v>82</v>
       </c>
       <c r="AP83" t="s" s="2">
         <v>82</v>
@@ -12200,10 +12244,10 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>555</v>
+        <v>508</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>555</v>
+        <v>508</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -12223,23 +12267,21 @@
         <v>82</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>392</v>
+        <v>500</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>556</v>
+        <v>509</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>394</v>
+        <v>510</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>557</v>
-      </c>
-      <c r="O84" t="s" s="2">
-        <v>396</v>
-      </c>
+        <v>503</v>
+      </c>
+      <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
         <v>82</v>
       </c>
@@ -12287,7 +12329,7 @@
         <v>82</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>555</v>
+        <v>508</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>80</v>
@@ -12296,36 +12338,36 @@
         <v>92</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>104</v>
+        <v>504</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>105</v>
+        <v>505</v>
       </c>
       <c r="AK84" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>558</v>
+        <v>82</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>399</v>
+        <v>506</v>
       </c>
       <c r="AN84" t="s" s="2">
-        <v>400</v>
+        <v>511</v>
       </c>
       <c r="AO84" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP84" t="s" s="2">
-        <v>401</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>559</v>
+        <v>512</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>559</v>
+        <v>512</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12339,7 +12381,7 @@
         <v>92</v>
       </c>
       <c r="H85" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I85" t="s" s="2">
         <v>82</v>
@@ -12351,16 +12393,16 @@
         <v>198</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>560</v>
+        <v>513</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>561</v>
+        <v>514</v>
       </c>
       <c r="N85" t="s" s="2">
-        <v>562</v>
+        <v>515</v>
       </c>
       <c r="O85" t="s" s="2">
-        <v>406</v>
+        <v>516</v>
       </c>
       <c r="P85" t="s" s="2">
         <v>82</v>
@@ -12385,11 +12427,13 @@
         <v>82</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="Y85" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="Y85" t="s" s="2">
+        <v>517</v>
+      </c>
       <c r="Z85" t="s" s="2">
-        <v>563</v>
+        <v>518</v>
       </c>
       <c r="AA85" t="s" s="2">
         <v>82</v>
@@ -12407,7 +12451,7 @@
         <v>82</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>559</v>
+        <v>512</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>80</v>
@@ -12416,7 +12460,7 @@
         <v>92</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>410</v>
+        <v>104</v>
       </c>
       <c r="AJ85" t="s" s="2">
         <v>105</v>
@@ -12425,13 +12469,13 @@
         <v>82</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>82</v>
+        <v>519</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>106</v>
+        <v>520</v>
       </c>
       <c r="AN85" t="s" s="2">
-        <v>411</v>
+        <v>436</v>
       </c>
       <c r="AO85" t="s" s="2">
         <v>82</v>
@@ -12442,14 +12486,14 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>564</v>
+        <v>521</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>564</v>
+        <v>521</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
-        <v>413</v>
+        <v>82</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" t="s" s="2">
@@ -12471,16 +12515,16 @@
         <v>198</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>414</v>
+        <v>522</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>415</v>
+        <v>523</v>
       </c>
       <c r="N86" t="s" s="2">
-        <v>416</v>
+        <v>524</v>
       </c>
       <c r="O86" t="s" s="2">
-        <v>417</v>
+        <v>525</v>
       </c>
       <c r="P86" t="s" s="2">
         <v>82</v>
@@ -12505,13 +12549,13 @@
         <v>82</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>407</v>
+        <v>341</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>418</v>
+        <v>526</v>
       </c>
       <c r="Z86" t="s" s="2">
-        <v>419</v>
+        <v>527</v>
       </c>
       <c r="AA86" t="s" s="2">
         <v>82</v>
@@ -12529,7 +12573,7 @@
         <v>82</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>564</v>
+        <v>521</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>80</v>
@@ -12547,27 +12591,27 @@
         <v>82</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>420</v>
+        <v>519</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>421</v>
+        <v>520</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP86" t="s" s="2">
-        <v>423</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>565</v>
+        <v>528</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>565</v>
+        <v>528</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12578,7 +12622,7 @@
         <v>80</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H87" t="s" s="2">
         <v>82</v>
@@ -12590,19 +12634,19 @@
         <v>82</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>83</v>
+        <v>529</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>566</v>
+        <v>530</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>567</v>
+        <v>531</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>473</v>
+        <v>532</v>
       </c>
       <c r="O87" t="s" s="2">
-        <v>474</v>
+        <v>533</v>
       </c>
       <c r="P87" t="s" s="2">
         <v>82</v>
@@ -12651,41 +12695,1491 @@
         <v>82</v>
       </c>
       <c r="AF87" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
+        <v>534</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL87" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM87" t="s" s="2">
+        <v>535</v>
+      </c>
+      <c r="AN87" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="AO87" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP87" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" hidden="true">
+      <c r="A88" t="s" s="2">
+        <v>537</v>
+      </c>
+      <c r="B88" t="s" s="2">
+        <v>537</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G88" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="N88" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="O88" s="2"/>
+      <c r="P88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q88" s="2"/>
+      <c r="R88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>537</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM88" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="AN88" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="AO88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP88" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" hidden="true">
+      <c r="A89" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="B89" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G89" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="M89" t="s" s="2">
+        <v>544</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="O89" s="2"/>
+      <c r="P89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q89" s="2"/>
+      <c r="R89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM89" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="AN89" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="AO89" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP89" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" hidden="true">
+      <c r="A90" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="B90" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G90" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J90" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K90" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="M90" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="N90" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="O90" s="2"/>
+      <c r="P90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q90" s="2"/>
+      <c r="R90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF90" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="AG90" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH90" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI90" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ90" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM90" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="AN90" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="AO90" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP90" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" hidden="true">
+      <c r="A91" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="B91" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G91" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>556</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="O91" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="P91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q91" s="2"/>
+      <c r="R91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM91" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="AN91" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="AO91" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP91" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" hidden="true">
+      <c r="A92" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="B92" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G92" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="M92" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q92" s="2"/>
+      <c r="R92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AN92" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AO92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP92" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" hidden="true">
+      <c r="A93" t="s" s="2">
+        <v>562</v>
+      </c>
+      <c r="B93" t="s" s="2">
+        <v>562</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="M93" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="N93" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="O93" s="2"/>
+      <c r="P93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q93" s="2"/>
+      <c r="R93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AN93" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AO93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP93" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="B94" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="O94" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="P94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q94" s="2"/>
+      <c r="R94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI94" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ94" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AN94" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AO94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP94" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="B95" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L95" t="s" s="2">
         <v>565</v>
       </c>
-      <c r="AG87" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH87" t="s" s="2">
+      <c r="M95" t="s" s="2">
+        <v>566</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>567</v>
+      </c>
+      <c r="O95" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="P95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q95" s="2"/>
+      <c r="R95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>568</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AN95" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AO95" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AP95" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="B96" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E96" s="2"/>
+      <c r="F96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>570</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="N96" t="s" s="2">
+        <v>571</v>
+      </c>
+      <c r="O96" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="P96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q96" s="2"/>
+      <c r="R96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>572</v>
+      </c>
+      <c r="AM96" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="AN96" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="AO96" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP96" t="s" s="2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="97" hidden="true">
+      <c r="A97" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="B97" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E97" s="2"/>
+      <c r="F97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="M97" t="s" s="2">
+        <v>575</v>
+      </c>
+      <c r="N97" t="s" s="2">
+        <v>576</v>
+      </c>
+      <c r="O97" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="P97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q97" s="2"/>
+      <c r="R97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="Y97" s="2"/>
+      <c r="Z97" t="s" s="2">
+        <v>577</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM97" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AN97" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AO97" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP97" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" hidden="true">
+      <c r="A98" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="B98" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="E98" s="2"/>
+      <c r="F98" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G98" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="AI87" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AJ87" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AK87" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL87" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AM87" t="s" s="2">
-        <v>476</v>
-      </c>
-      <c r="AN87" t="s" s="2">
-        <v>477</v>
-      </c>
-      <c r="AO87" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP87" t="s" s="2">
+      <c r="H98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L98" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="M98" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="N98" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="O98" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="P98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q98" s="2"/>
+      <c r="R98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X98" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="Y98" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="Z98" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL98" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="AM98" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="AN98" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="AO98" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP98" t="s" s="2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="99" hidden="true">
+      <c r="A99" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="B99" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E99" s="2"/>
+      <c r="F99" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G99" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K99" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="L99" t="s" s="2">
+        <v>580</v>
+      </c>
+      <c r="M99" t="s" s="2">
+        <v>581</v>
+      </c>
+      <c r="N99" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="O99" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="P99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q99" s="2"/>
+      <c r="R99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Y99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF99" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="AG99" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH99" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AK99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM99" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="AN99" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AO99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP99" t="s" s="2">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP87">
+  <autoFilter ref="A1:AP99">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -12695,7 +14189,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI86">
+  <conditionalFormatting sqref="A2:AI98">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>